<commit_message>
added fixed GPA cal/Result upload system
</commit_message>
<xml_diff>
--- a/result/test.xlsx
+++ b/result/test.xlsx
@@ -15,54 +15,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>2012CS1</t>
   </si>
   <si>
+    <t>C-</t>
+  </si>
+  <si>
+    <t>2012CS2</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>2012CS3</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>2012CS4</t>
+  </si>
+  <si>
+    <t>B-</t>
+  </si>
+  <si>
+    <t>2012CS5</t>
+  </si>
+  <si>
+    <t>2012CS6</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>2012CS7</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>2012CS8</t>
+  </si>
+  <si>
     <t>A+</t>
   </si>
   <si>
-    <t>2012CS2</t>
+    <t>2012CS9</t>
   </si>
   <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>2012CS3</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>2012CS4</t>
-  </si>
-  <si>
-    <t>B-</t>
-  </si>
-  <si>
-    <t>2012CS5</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>2012CS6</t>
-  </si>
-  <si>
-    <t>AB</t>
-  </si>
-  <si>
-    <t>2012CS7</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>2012CS8</t>
-  </si>
-  <si>
-    <t>2012CS9</t>
   </si>
   <si>
     <t>2012CS10</t>
@@ -80,6 +83,7 @@
       <sz val="10"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -139,8 +143,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -164,89 +172,92 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.63839285714286"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>